<commit_message>
implemented new partition method - link process method
</commit_message>
<xml_diff>
--- a/r_map/data_egrid_emf_As.xlsx
+++ b/r_map/data_egrid_emf_As.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14985" windowHeight="6825"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19905" windowHeight="6810"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -435,9 +435,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21:D21"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -461,85 +459,47 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B2">
-        <v>0</v>
-      </c>
-      <c r="C2">
-        <v>0</v>
-      </c>
-      <c r="D2">
-        <v>0</v>
-      </c>
-    </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
-      <c r="B3">
-        <v>0</v>
-      </c>
-      <c r="C3">
-        <v>0</v>
-      </c>
-      <c r="D3">
-        <v>0</v>
-      </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
-      <c r="B4">
-        <v>0</v>
-      </c>
-      <c r="C4">
-        <v>0</v>
-      </c>
-      <c r="D4">
-        <v>0</v>
-      </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
       <c r="B5">
-        <v>0</v>
+        <v>1121.6475366560899</v>
       </c>
       <c r="C5">
-        <v>0</v>
+        <v>0.45866400042399974</v>
       </c>
       <c r="D5">
-        <v>0</v>
+        <v>12.735575250268212</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
-      <c r="B6">
-        <v>0</v>
-      </c>
-      <c r="C6">
-        <v>0</v>
-      </c>
-      <c r="D6">
-        <v>0</v>
-      </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>5</v>
       </c>
       <c r="B7">
-        <v>2419.2191551329238</v>
+        <v>2397.4469980336244</v>
       </c>
       <c r="C7">
-        <v>0.12777098831577546</v>
+        <v>0.16629701509286393</v>
       </c>
       <c r="D7">
-        <v>3.7370505550693451</v>
+        <v>3.4675820974288225</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -547,55 +507,37 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>2812.9596952487791</v>
+        <v>2804.8673341435751</v>
       </c>
       <c r="C8">
-        <v>0.13282417709981051</v>
+        <v>0.24632350762520833</v>
       </c>
       <c r="D8">
-        <v>4.5863280332712835</v>
+        <v>5.2791067366499052</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>7</v>
       </c>
-      <c r="B9">
-        <v>0</v>
-      </c>
-      <c r="C9">
-        <v>0</v>
-      </c>
-      <c r="D9">
-        <v>0</v>
-      </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>8</v>
       </c>
-      <c r="B10">
-        <v>0</v>
-      </c>
-      <c r="C10">
-        <v>0</v>
-      </c>
-      <c r="D10">
-        <v>0</v>
-      </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>9</v>
       </c>
       <c r="B11">
-        <v>1078.4121933398442</v>
+        <v>1046.7037338972473</v>
       </c>
       <c r="C11">
         <v>0</v>
       </c>
       <c r="D11">
-        <v>186.80031295621546</v>
+        <v>122.69366375369066</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -603,83 +545,56 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>1132.8490994067702</v>
+        <v>1271.3509444178469</v>
       </c>
       <c r="C12">
-        <v>0.32966171594392746</v>
+        <v>0</v>
       </c>
       <c r="D12">
-        <v>139.0570551314251</v>
+        <v>110.29082062794942</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>11</v>
       </c>
-      <c r="B13">
-        <v>0</v>
-      </c>
-      <c r="C13">
-        <v>0</v>
-      </c>
-      <c r="D13">
-        <v>0</v>
-      </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>12</v>
       </c>
       <c r="B14">
-        <v>1091.2984859118972</v>
+        <v>1105.688290913879</v>
       </c>
       <c r="C14">
-        <v>6.1751677021090731E-2</v>
+        <v>1.4137397268505738E-2</v>
       </c>
       <c r="D14">
-        <v>115.19004111822326</v>
+        <v>33.298787647873297</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>13</v>
       </c>
-      <c r="B15">
-        <v>0</v>
-      </c>
-      <c r="C15">
-        <v>0</v>
-      </c>
-      <c r="D15">
-        <v>0</v>
-      </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>14</v>
       </c>
-      <c r="B16">
-        <v>0</v>
-      </c>
-      <c r="C16">
-        <v>0</v>
-      </c>
-      <c r="D16">
-        <v>0</v>
-      </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>15</v>
       </c>
       <c r="B17">
-        <v>5632.1745357733398</v>
+        <v>5618.8865103340195</v>
       </c>
       <c r="C17">
-        <v>0.29248934600350512</v>
+        <v>0.3987294610427321</v>
       </c>
       <c r="D17">
-        <v>6.9941655313570523</v>
+        <v>7.3607681001160614</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -687,13 +602,13 @@
         <v>16</v>
       </c>
       <c r="B18">
-        <v>5500.3486655212346</v>
+        <v>5437.4721692008497</v>
       </c>
       <c r="C18">
-        <v>0.29603958705060746</v>
+        <v>0.27168383974023569</v>
       </c>
       <c r="D18">
-        <v>141.12735216743064</v>
+        <v>114.53607911419446</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -701,13 +616,13 @@
         <v>17</v>
       </c>
       <c r="B19">
-        <v>1452.694086178293</v>
+        <v>1513.6501832768045</v>
       </c>
       <c r="C19">
-        <v>0.13768899938936063</v>
+        <v>0</v>
       </c>
       <c r="D19">
-        <v>146.4778276970068</v>
+        <v>115.58767172313233</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -715,13 +630,13 @@
         <v>18</v>
       </c>
       <c r="B20">
-        <v>4028.700214152826</v>
+        <v>4191.22098253287</v>
       </c>
       <c r="C20">
-        <v>0.22911358696760745</v>
+        <v>0.30209940341538127</v>
       </c>
       <c r="D20">
-        <v>8.7137901629899872</v>
+        <v>13.90957656407797</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -729,13 +644,13 @@
         <v>19</v>
       </c>
       <c r="B21">
-        <v>0</v>
+        <v>1212.4220897554305</v>
       </c>
       <c r="C21">
-        <v>0</v>
+        <v>0.15206429208480401</v>
       </c>
       <c r="D21">
-        <v>0</v>
+        <v>186.15377694624723</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -743,13 +658,13 @@
         <v>20</v>
       </c>
       <c r="B22">
-        <v>1163.0651754465221</v>
+        <v>1177.2640827934172</v>
       </c>
       <c r="C22">
-        <v>7.8527036547241039E-2</v>
+        <v>0</v>
       </c>
       <c r="D22">
-        <v>123.93220346095688</v>
+        <v>102.23883301566036</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -757,13 +672,13 @@
         <v>21</v>
       </c>
       <c r="B23">
-        <v>1066.9938966080795</v>
+        <v>1118.6139578295308</v>
       </c>
       <c r="C23">
-        <v>0.19130997388736096</v>
+        <v>0</v>
       </c>
       <c r="D23">
-        <v>159.38187662210208</v>
+        <v>129.294262896541</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
@@ -771,13 +686,13 @@
         <v>22</v>
       </c>
       <c r="B24">
-        <v>1143.3239908483383</v>
+        <v>1168.6301357915765</v>
       </c>
       <c r="C24">
         <v>0</v>
       </c>
       <c r="D24">
-        <v>193.9725682632789</v>
+        <v>148.94582454163896</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -785,13 +700,13 @@
         <v>23</v>
       </c>
       <c r="B25">
-        <v>1125.6210000564597</v>
+        <v>1135.6928285138029</v>
       </c>
       <c r="C25">
-        <v>0.1012485157420745</v>
+        <v>0</v>
       </c>
       <c r="D25">
-        <v>175.16591353332882</v>
+        <v>133.45201597622855</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
@@ -799,13 +714,13 @@
         <v>24</v>
       </c>
       <c r="B26">
-        <v>2558.367947046987</v>
+        <v>3186.3252935344699</v>
       </c>
       <c r="C26">
-        <v>0.17057046589393166</v>
+        <v>0.32107660708224106</v>
       </c>
       <c r="D26">
-        <v>13.259241766734227</v>
+        <v>62.455109968727967</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
@@ -813,13 +728,13 @@
         <v>25</v>
       </c>
       <c r="B27">
-        <v>5219.2500087002445</v>
+        <v>5277.355990070364</v>
       </c>
       <c r="C27">
-        <v>0.28416905940597675</v>
+        <v>0.41716555524737875</v>
       </c>
       <c r="D27">
-        <v>11.492125457871889</v>
+        <v>12.828637181894603</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
@@ -827,13 +742,13 @@
         <v>26</v>
       </c>
       <c r="B28">
-        <v>5217.2576971377221</v>
+        <v>5170.9245420112675</v>
       </c>
       <c r="C28">
-        <v>0.28176715132997271</v>
+        <v>0.43591084833337845</v>
       </c>
       <c r="D28">
-        <v>10.277121048361494</v>
+        <v>11.82596964423858</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added: 1) plants that purchase coal from states w/o Cl coal samples are included by using basin-level data and 2) air pollution controls without many studies use sample level data for each study instead of averaged data
</commit_message>
<xml_diff>
--- a/r_map/data_egrid_emf_As.xlsx
+++ b/r_map/data_egrid_emf_As.xlsx
@@ -474,13 +474,13 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>13.4133266137753</v>
+        <v>21.474557569998417</v>
       </c>
       <c r="C5">
-        <v>1.6615388127017398E-3</v>
+        <v>1.1139371050135263E-3</v>
       </c>
       <c r="D5">
-        <v>3.551512420339932E-2</v>
+        <v>3.3862719637723124E-2</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -493,13 +493,13 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>103.04134659209438</v>
+        <v>143.37057952933651</v>
       </c>
       <c r="C7">
-        <v>8.9688427267222339E-3</v>
+        <v>7.7543764636170166E-3</v>
       </c>
       <c r="D7">
-        <v>5.8512140324020248</v>
+        <v>4.0946274621723573</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -507,13 +507,13 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>107.18904048327813</v>
+        <v>73.146974683871193</v>
       </c>
       <c r="C8">
-        <v>5.7050094697372001E-3</v>
+        <v>3.8028852378157933E-3</v>
       </c>
       <c r="D8">
-        <v>1.2620154565463195</v>
+        <v>1.1548169749744757</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -531,13 +531,13 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>15.172265319927243</v>
+        <v>26.379459841225277</v>
       </c>
       <c r="C11">
-        <v>5.7755050555109591E-4</v>
+        <v>1.2907434249125433E-3</v>
       </c>
       <c r="D11">
-        <v>0.70038464050956661</v>
+        <v>0.56614439437360864</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -545,13 +545,13 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>169.20631933846897</v>
+        <v>242.02123048820144</v>
       </c>
       <c r="C12">
-        <v>9.8356698275528977E-3</v>
+        <v>2.1231579893888516E-2</v>
       </c>
       <c r="D12">
-        <v>3.4618629466157214</v>
+        <v>3.1185722888937435</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -564,13 +564,13 @@
         <v>12</v>
       </c>
       <c r="B14">
-        <v>128.32336925006732</v>
+        <v>161.21288435241371</v>
       </c>
       <c r="C14">
-        <v>7.2670020744946429E-3</v>
+        <v>4.5729101723336373E-3</v>
       </c>
       <c r="D14">
-        <v>1.0440624022049168</v>
+        <v>0.97331036621811218</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -588,13 +588,13 @@
         <v>15</v>
       </c>
       <c r="B17">
-        <v>22.200185634078924</v>
+        <v>15.380522610799117</v>
       </c>
       <c r="C17">
-        <v>1.8423154879788857E-2</v>
+        <v>1.9072841271542879E-4</v>
       </c>
       <c r="D17">
-        <v>0.47308634515264303</v>
+        <v>9.8111181622800803E-2</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -602,13 +602,13 @@
         <v>16</v>
       </c>
       <c r="B18">
-        <v>161.09476130796733</v>
+        <v>142.06463302404146</v>
       </c>
       <c r="C18">
-        <v>4.1840544910831182E-3</v>
+        <v>2.8652528870556069E-3</v>
       </c>
       <c r="D18">
-        <v>7.0700967237073886</v>
+        <v>4.6013404844227663</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -616,13 +616,13 @@
         <v>17</v>
       </c>
       <c r="B19">
-        <v>156.28493648011718</v>
+        <v>102.59925455126825</v>
       </c>
       <c r="C19">
-        <v>5.1729385348202482E-3</v>
+        <v>3.4177471067292839E-3</v>
       </c>
       <c r="D19">
-        <v>5.9668455055760061</v>
+        <v>3.7123626844809352</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -630,13 +630,13 @@
         <v>18</v>
       </c>
       <c r="B20">
-        <v>1179.5102111569222</v>
+        <v>749.15912282950364</v>
       </c>
       <c r="C20">
-        <v>9.9132876628876571E-2</v>
+        <v>5.8255920862844736E-2</v>
       </c>
       <c r="D20">
-        <v>18.936228907481972</v>
+        <v>10.025801934582807</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -644,13 +644,13 @@
         <v>19</v>
       </c>
       <c r="B21">
-        <v>16.79694362006747</v>
+        <v>144.1690614397111</v>
       </c>
       <c r="C21">
-        <v>9.6293317599829072E-4</v>
+        <v>7.5804305098319223E-3</v>
       </c>
       <c r="D21">
-        <v>0.29446627408051268</v>
+        <v>0.15834694711400502</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -658,13 +658,13 @@
         <v>20</v>
       </c>
       <c r="B22">
-        <v>9.8566313313667386</v>
+        <v>36.462789248376531</v>
       </c>
       <c r="C22">
-        <v>3.0992328239202337E-4</v>
+        <v>4.0007976612425747E-4</v>
       </c>
       <c r="D22">
-        <v>0.82557572614867492</v>
+        <v>0.55965815643999217</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -672,13 +672,13 @@
         <v>21</v>
       </c>
       <c r="B23">
-        <v>157.93570949823342</v>
+        <v>121.61017387057332</v>
       </c>
       <c r="C23">
-        <v>4.6158647254689031E-2</v>
+        <v>2.9927953734358855E-2</v>
       </c>
       <c r="D23">
-        <v>4.5681723753020043</v>
+        <v>3.2429363691050894</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
@@ -686,13 +686,13 @@
         <v>22</v>
       </c>
       <c r="B24">
-        <v>69.652735435237545</v>
+        <v>45.928649848411027</v>
       </c>
       <c r="C24">
-        <v>4.535140423012448E-3</v>
+        <v>3.0200931189827709E-3</v>
       </c>
       <c r="D24">
-        <v>7.7434068268624243E-2</v>
+        <v>8.7749705103078959E-2</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -700,13 +700,13 @@
         <v>23</v>
       </c>
       <c r="B25">
-        <v>81.8264172319073</v>
+        <v>74.721363344339252</v>
       </c>
       <c r="C25">
-        <v>1.2533746715075959E-3</v>
+        <v>8.3189264424682059E-4</v>
       </c>
       <c r="D25">
-        <v>6.417859515720628</v>
+        <v>3.9416560952647228</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
@@ -714,13 +714,13 @@
         <v>24</v>
       </c>
       <c r="B26">
-        <v>416.44570418955772</v>
+        <v>323.99435838102909</v>
       </c>
       <c r="C26">
-        <v>5.4397597041174431E-2</v>
+        <v>3.4819671609657897E-2</v>
       </c>
       <c r="D26">
-        <v>32.459020443473008</v>
+        <v>20.86122161132851</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
@@ -728,13 +728,13 @@
         <v>25</v>
       </c>
       <c r="B27">
-        <v>375.44714188058316</v>
+        <v>361.5578598943535</v>
       </c>
       <c r="C27">
-        <v>2.8809118384815063E-2</v>
+        <v>1.823919178431959E-2</v>
       </c>
       <c r="D27">
-        <v>3.039775168031901</v>
+        <v>1.8834472767064019</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
@@ -742,13 +742,13 @@
         <v>26</v>
       </c>
       <c r="B28">
-        <v>216.2911153880159</v>
+        <v>192.15111546133838</v>
       </c>
       <c r="C28">
-        <v>1.2366037097810784E-2</v>
+        <v>6.7217245421593332E-3</v>
       </c>
       <c r="D28">
-        <v>0.52955117152995668</v>
+        <v>0.41427121391883531</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
All code revisions for paper resubmission and added descriptions in each script
</commit_message>
<xml_diff>
--- a/r_map/data_egrid_emf_As.xlsx
+++ b/r_map/data_egrid_emf_As.xlsx
@@ -474,13 +474,13 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>21.474557569998417</v>
+        <v>21.520206429768169</v>
       </c>
       <c r="C5">
-        <v>1.1139371050135263E-3</v>
+        <v>1.1272432183035044E-3</v>
       </c>
       <c r="D5">
-        <v>3.3862719637723124E-2</v>
+        <v>3.4090926552876433E-2</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -493,13 +493,13 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>143.37057952933651</v>
+        <v>145.72917917316062</v>
       </c>
       <c r="C7">
-        <v>7.7543764636170166E-3</v>
+        <v>7.7814463573146224E-3</v>
       </c>
       <c r="D7">
-        <v>4.0946274621723573</v>
+        <v>4.12498375402234</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -507,13 +507,13 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>73.146974683871193</v>
+        <v>71.946019900233679</v>
       </c>
       <c r="C8">
-        <v>3.8028852378157933E-3</v>
+        <v>3.6695335952044608E-3</v>
       </c>
       <c r="D8">
-        <v>1.1548169749744757</v>
+        <v>1.1442108399850954</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -531,13 +531,13 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>26.379459841225277</v>
+        <v>26.353638430584944</v>
       </c>
       <c r="C11">
-        <v>1.2907434249125433E-3</v>
+        <v>1.2875277280630219E-3</v>
       </c>
       <c r="D11">
-        <v>0.56614439437360864</v>
+        <v>0.56026176916531156</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -545,13 +545,13 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>242.02123048820144</v>
+        <v>241.47480555681909</v>
       </c>
       <c r="C12">
-        <v>2.1231579893888516E-2</v>
+        <v>2.1214001186750386E-2</v>
       </c>
       <c r="D12">
-        <v>3.1185722888937435</v>
+        <v>3.0996893751342629</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -564,13 +564,13 @@
         <v>12</v>
       </c>
       <c r="B14">
-        <v>161.21288435241371</v>
+        <v>160.93485352155639</v>
       </c>
       <c r="C14">
-        <v>4.5729101723336373E-3</v>
+        <v>4.7031965299132814E-3</v>
       </c>
       <c r="D14">
-        <v>0.97331036621811218</v>
+        <v>0.97127993464041784</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -588,13 +588,13 @@
         <v>15</v>
       </c>
       <c r="B17">
-        <v>15.380522610799117</v>
+        <v>15.38018283959266</v>
       </c>
       <c r="C17">
-        <v>1.9072841271542879E-4</v>
+        <v>1.9320469006327113E-4</v>
       </c>
       <c r="D17">
-        <v>9.8111181622800803E-2</v>
+        <v>9.7974555740671918E-2</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -602,13 +602,13 @@
         <v>16</v>
       </c>
       <c r="B18">
-        <v>142.06463302404146</v>
+        <v>141.33939009595125</v>
       </c>
       <c r="C18">
-        <v>2.8652528870556069E-3</v>
+        <v>2.932115208409857E-3</v>
       </c>
       <c r="D18">
-        <v>4.6013404844227663</v>
+        <v>4.6952245564774167</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -616,13 +616,13 @@
         <v>17</v>
       </c>
       <c r="B19">
-        <v>102.59925455126825</v>
+        <v>104.23981899114571</v>
       </c>
       <c r="C19">
-        <v>3.4177471067292839E-3</v>
+        <v>3.3873052600669109E-3</v>
       </c>
       <c r="D19">
-        <v>3.7123626844809352</v>
+        <v>3.800373945194869</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -630,13 +630,13 @@
         <v>18</v>
       </c>
       <c r="B20">
-        <v>749.15912282950364</v>
+        <v>752.33952780887466</v>
       </c>
       <c r="C20">
-        <v>5.8255920862844736E-2</v>
+        <v>5.839623010934774E-2</v>
       </c>
       <c r="D20">
-        <v>10.025801934582807</v>
+        <v>10.014934153863225</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -644,13 +644,13 @@
         <v>19</v>
       </c>
       <c r="B21">
-        <v>144.1690614397111</v>
+        <v>143.97121119104895</v>
       </c>
       <c r="C21">
-        <v>7.5804305098319223E-3</v>
+        <v>7.5498650666191176E-3</v>
       </c>
       <c r="D21">
-        <v>0.15834694711400502</v>
+        <v>0.16163370068992983</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -658,13 +658,13 @@
         <v>20</v>
       </c>
       <c r="B22">
-        <v>36.462789248376531</v>
+        <v>36.161601433196672</v>
       </c>
       <c r="C22">
-        <v>4.0007976612425747E-4</v>
+        <v>3.9709150907122828E-4</v>
       </c>
       <c r="D22">
-        <v>0.55965815643999217</v>
+        <v>0.56180494979280005</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -672,13 +672,13 @@
         <v>21</v>
       </c>
       <c r="B23">
-        <v>121.61017387057332</v>
+        <v>122.91463655673859</v>
       </c>
       <c r="C23">
-        <v>2.9927953734358855E-2</v>
+        <v>2.9832594242725372E-2</v>
       </c>
       <c r="D23">
-        <v>3.2429363691050894</v>
+        <v>3.1827066411180329</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
@@ -686,13 +686,13 @@
         <v>22</v>
       </c>
       <c r="B24">
-        <v>45.928649848411027</v>
+        <v>46.67067872076769</v>
       </c>
       <c r="C24">
-        <v>3.0200931189827709E-3</v>
+        <v>3.0501812916502139E-3</v>
       </c>
       <c r="D24">
-        <v>8.7749705103078959E-2</v>
+        <v>8.8455329328260626E-2</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -700,13 +700,13 @@
         <v>23</v>
       </c>
       <c r="B25">
-        <v>74.721363344339252</v>
+        <v>74.50731997421083</v>
       </c>
       <c r="C25">
-        <v>8.3189264424682059E-4</v>
+        <v>8.3609681352537157E-4</v>
       </c>
       <c r="D25">
-        <v>3.9416560952647228</v>
+        <v>3.951687710765011</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
@@ -714,13 +714,13 @@
         <v>24</v>
       </c>
       <c r="B26">
-        <v>323.99435838102909</v>
+        <v>324.58605414982742</v>
       </c>
       <c r="C26">
-        <v>3.4819671609657897E-2</v>
+        <v>3.496528360998933E-2</v>
       </c>
       <c r="D26">
-        <v>20.86122161132851</v>
+        <v>21.154454951072182</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
@@ -728,13 +728,13 @@
         <v>25</v>
       </c>
       <c r="B27">
-        <v>361.5578598943535</v>
+        <v>362.79386483199693</v>
       </c>
       <c r="C27">
-        <v>1.823919178431959E-2</v>
+        <v>1.8418729310806414E-2</v>
       </c>
       <c r="D27">
-        <v>1.8834472767064019</v>
+        <v>1.8770543216539868</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
@@ -742,13 +742,13 @@
         <v>26</v>
       </c>
       <c r="B28">
-        <v>192.15111546133838</v>
+        <v>192.5972061419902</v>
       </c>
       <c r="C28">
-        <v>6.7217245421593332E-3</v>
+        <v>6.6441124709802363E-3</v>
       </c>
       <c r="D28">
-        <v>0.41427121391883531</v>
+        <v>0.41136444828102653</v>
       </c>
     </row>
   </sheetData>

</xml_diff>